<commit_message>
dynamics ics endpoints and pwd hashing back on site
</commit_message>
<xml_diff>
--- a/backend/all_events.xlsx
+++ b/backend/all_events.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthieu/projects/cafe2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthieu/projects/cafe2.0/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230FD0D5-D4BF-CE45-B00F-5304391420B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C525DF7-842A-6649-AD02-274D09B6D7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="900" windowWidth="14480" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="124">
   <si>
     <t>start</t>
   </si>
@@ -250,7 +250,148 @@
     <t>Leçon Ehe</t>
   </si>
   <si>
-    <t>Leçon TR</t>
+    <t>2025-12-08T08:00</t>
+  </si>
+  <si>
+    <t>2025-12-09T13:30</t>
+  </si>
+  <si>
+    <t>2025-12-08T13:30</t>
+  </si>
+  <si>
+    <t>2025-12-09T08:30</t>
+  </si>
+  <si>
+    <t>2025-12-10T08:00</t>
+  </si>
+  <si>
+    <t>2025-12-10T13:30</t>
+  </si>
+  <si>
+    <t>2025-12-11T08:00</t>
+  </si>
+  <si>
+    <t>2025-12-12T08:00</t>
+  </si>
+  <si>
+    <t>2025-12-12T13:30</t>
+  </si>
+  <si>
+    <t>2025-12-15T08:00</t>
+  </si>
+  <si>
+    <t>2025-12-15T13:30</t>
+  </si>
+  <si>
+    <t>2025-12-16T08:30</t>
+  </si>
+  <si>
+    <t>2025-12-16T13:30</t>
+  </si>
+  <si>
+    <t>2025-12-17T08:00</t>
+  </si>
+  <si>
+    <t>2025-12-17T13:30</t>
+  </si>
+  <si>
+    <t>2025-12-18T08:00</t>
+  </si>
+  <si>
+    <t>2025-12-19T08:00</t>
+  </si>
+  <si>
+    <t>2025-12-19T13:30</t>
+  </si>
+  <si>
+    <t>2025-12-08T12:15</t>
+  </si>
+  <si>
+    <t>2025-12-08T17:45</t>
+  </si>
+  <si>
+    <t>2025-12-09T12:15</t>
+  </si>
+  <si>
+    <t>2025-12-09T17:45</t>
+  </si>
+  <si>
+    <t>2025-12-10T12:15</t>
+  </si>
+  <si>
+    <t>2025-12-10T17:45</t>
+  </si>
+  <si>
+    <t>2025-12-11T12:15</t>
+  </si>
+  <si>
+    <t>2025-12-12T12:15</t>
+  </si>
+  <si>
+    <t>2025-12-12T17:45</t>
+  </si>
+  <si>
+    <t>2025-12-15T12:15</t>
+  </si>
+  <si>
+    <t>2025-12-15T17:45</t>
+  </si>
+  <si>
+    <t>2025-12-16T12:15</t>
+  </si>
+  <si>
+    <t>2025-12-16T17:45</t>
+  </si>
+  <si>
+    <t>2025-12-17T12:15</t>
+  </si>
+  <si>
+    <t>2025-12-17T17:45</t>
+  </si>
+  <si>
+    <t>2025-12-18T12:15</t>
+  </si>
+  <si>
+    <t>2025-12-19T12:15</t>
+  </si>
+  <si>
+    <t>2025-12-19T17:45</t>
+  </si>
+  <si>
+    <t>Leçon com. AJ</t>
+  </si>
+  <si>
+    <t>Ondel TR</t>
+  </si>
+  <si>
+    <t>Exam EN Telecom</t>
+  </si>
+  <si>
+    <t>Sys ML SM</t>
+  </si>
+  <si>
+    <t>Exam EN Fond</t>
+  </si>
+  <si>
+    <t>Auto JPO</t>
+  </si>
+  <si>
+    <t>Leçon FA</t>
+  </si>
+  <si>
+    <t>En Telecom JSM</t>
+  </si>
+  <si>
+    <t>Visite</t>
+  </si>
+  <si>
+    <t>TS/Ondel Exam CD</t>
+  </si>
+  <si>
+    <t>Python JO</t>
+  </si>
+  <si>
+    <t>Exam OS PV</t>
   </si>
 </sst>
 </file>
@@ -590,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="116" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1080,7 +1221,7 @@
         <v>55</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1166,13 +1307,13 @@
         <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E25">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1192,15 +1333,429 @@
         <v>58</v>
       </c>
       <c r="D26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
         <v>55</v>
       </c>
-      <c r="E26">
+      <c r="E29">
         <v>7</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30">
+        <v>8</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31">
+        <v>9</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36">
+        <v>11</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38">
+        <v>7</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39">
+        <v>8</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41">
+        <v>12</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42">
+        <v>13</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43">
+        <v>7</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44">
+        <v>7</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
         <v>1</v>
       </c>
     </row>

</xml_diff>